<commit_message>
Zeitmessung für den Vergleich der alternativen Szenario Funktion (alte Zeitmessungen sind ungültig)
</commit_message>
<xml_diff>
--- a/Zeitmessungen urbs.xlsx
+++ b/Zeitmessungen urbs.xlsx
@@ -1654,7 +1654,7 @@
   <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,20 +1944,20 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="24">
-        <f>SUM(A4:A103)/COUNT(A4:A103)</f>
-        <v>2.6734374999999999</v>
+        <f>SUM(A4:A103)/COUNT(A4:A103)/10</f>
+        <v>0.26734374999999999</v>
       </c>
       <c r="B105" s="24">
-        <f>SUM(B4:B103)/COUNT(B4:B103)</f>
-        <v>0.53281250000000002</v>
+        <f>SUM(B4:B103)/COUNT(B4:B103)/100</f>
+        <v>5.3281250000000004E-3</v>
       </c>
       <c r="E105" s="24">
         <f>SUM(E4:E103)/COUNT(E4:E103)</f>
         <v>10.734375</v>
       </c>
       <c r="F105" s="24">
-        <f>SUM(F4:F103)/COUNT(F4:F103)</f>
-        <v>1.346875</v>
+        <f>SUM(F4:F103)/COUNT(F4:F103)/10</f>
+        <v>0.13468750000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Verwendung von prob.del_component(): Zeitlich kein Vorteil, aber keine Fehlermeldungen mehr.
</commit_message>
<xml_diff>
--- a/Zeitmessungen urbs.xlsx
+++ b/Zeitmessungen urbs.xlsx
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="123">
   <si>
     <t>3 Modelle gescheitert (file signature not found;  Unable to open/create file 'result\mimo-example-20181002T1210\scenario_base.h5'</t>
   </si>
@@ -539,9 +539,6 @@
     <t>prob=alternative_scenario_stock_prices(prob_base)</t>
   </si>
   <si>
-    <t>Vergleich normales Szenario zu alternativem Szenario mit nur zwei Zeitschritten</t>
-  </si>
-  <si>
     <t>Zeit pro 100 alternative Szenarien:</t>
   </si>
   <si>
@@ -555,6 +552,15 @@
   </si>
   <si>
     <t>Zeit pro 10 alternative Szenarien in s:</t>
+  </si>
+  <si>
+    <t>Vergleich normales Szenario zu alternativem Szenario mit nur drei Zeitschritten</t>
+  </si>
+  <si>
+    <t>Verwendung von prob.del_component() in Szenario (vermeidet Fehlermeldungen):</t>
+  </si>
+  <si>
+    <t>Zeit pro 10 alternative Szenarien:</t>
   </si>
 </sst>
 </file>
@@ -628,7 +634,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -716,12 +722,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -752,7 +778,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1651,313 +1679,338 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.85546875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" style="24" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="24"/>
+    <col min="2" max="2" width="47.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="24"/>
     <col min="5" max="5" width="71.85546875" style="24" customWidth="1"/>
     <col min="6" max="6" width="47.140625" style="24" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="24"/>
+    <col min="7" max="7" width="49.7109375" style="24" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="C4" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="24">
-        <v>2.703125</v>
-      </c>
-      <c r="B4" s="24">
-        <v>0.546875</v>
-      </c>
-      <c r="E4" s="24">
-        <v>10.78125</v>
-      </c>
-      <c r="F4" s="24">
-        <v>1.359375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
-        <v>2.671875</v>
+        <v>2.609375</v>
       </c>
       <c r="B5" s="24">
-        <v>0.53125</v>
-      </c>
+        <v>0.46875</v>
+      </c>
+      <c r="C5" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="28"/>
       <c r="E5" s="24">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="F5" s="24">
-        <v>1.359375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.21875</v>
+      </c>
+      <c r="G5" s="24">
+        <v>1.234375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
-        <v>2.671875</v>
+        <v>2.609375</v>
       </c>
       <c r="B6" s="24">
         <v>0.515625</v>
       </c>
+      <c r="C6" s="24">
+        <v>0.484375</v>
+      </c>
+      <c r="D6" s="28"/>
       <c r="E6" s="24">
-        <v>10.6875</v>
+        <v>8.53125</v>
       </c>
       <c r="F6" s="24">
-        <v>1.421875</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.15625</v>
+      </c>
+      <c r="G6" s="24">
+        <v>1.203125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
+        <v>2.703125</v>
+      </c>
+      <c r="B7" s="24">
+        <v>0.515625</v>
+      </c>
+      <c r="C7" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="24">
+        <v>9.15625</v>
+      </c>
+      <c r="F7" s="24">
+        <v>1.21875</v>
+      </c>
+      <c r="G7" s="24">
+        <v>1.21875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
         <v>2.671875</v>
       </c>
-      <c r="B7" s="24">
-        <v>0.53125</v>
-      </c>
-      <c r="E7" s="24">
-        <v>11.34375</v>
-      </c>
-      <c r="F7" s="24">
-        <v>1.328125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="24">
-        <v>2.65625</v>
-      </c>
       <c r="B8" s="24">
-        <v>0.53125</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="28"/>
       <c r="E8" s="24">
-        <v>10.484375</v>
+        <v>9.125</v>
       </c>
       <c r="F8" s="24">
-        <v>1.3125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.296875</v>
+      </c>
+      <c r="G8" s="24">
+        <v>1.234375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
-        <v>2.625</v>
+        <v>2.5625</v>
       </c>
       <c r="B9" s="24">
-        <v>0.53125</v>
-      </c>
+        <v>0.515625</v>
+      </c>
+      <c r="C9" s="24">
+        <v>0.484375</v>
+      </c>
+      <c r="D9" s="28"/>
       <c r="E9" s="24">
-        <v>10.53125</v>
+        <v>9.59375</v>
       </c>
       <c r="F9" s="24">
-        <v>1.328125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.203125</v>
+      </c>
+      <c r="G9" s="24">
+        <v>1.203125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
-        <v>2.65625</v>
+        <v>2.640625</v>
       </c>
       <c r="B10" s="24">
-        <v>0.53125</v>
-      </c>
+        <v>0.515625</v>
+      </c>
+      <c r="C10" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="28"/>
       <c r="E10" s="24">
-        <v>10.515625</v>
+        <v>8.875</v>
       </c>
       <c r="F10" s="24">
-        <v>1.3125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.203125</v>
+      </c>
+      <c r="G10" s="24">
+        <v>1.15625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
+        <v>2.671875</v>
+      </c>
+      <c r="B11" s="24">
+        <v>0.515625</v>
+      </c>
+      <c r="C11" s="24">
+        <v>0.484375</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="24">
+        <v>9.140625</v>
+      </c>
+      <c r="F11" s="24">
+        <v>1.140625</v>
+      </c>
+      <c r="G11" s="24">
+        <v>1.234375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>2.796875</v>
+      </c>
+      <c r="B12" s="24">
+        <v>0.515625</v>
+      </c>
+      <c r="C12" s="24">
+        <v>0.484375</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="24">
+        <v>9.296875</v>
+      </c>
+      <c r="F12" s="24">
+        <v>1.109375</v>
+      </c>
+      <c r="G12" s="24">
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>2.5625</v>
+      </c>
+      <c r="B13" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="24">
+        <v>9.203125</v>
+      </c>
+      <c r="F13" s="24">
+        <v>1.15625</v>
+      </c>
+      <c r="G13" s="24">
+        <v>1.296875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
         <v>2.609375</v>
       </c>
-      <c r="B11" s="24">
-        <v>0.546875</v>
-      </c>
-      <c r="E11" s="24">
-        <v>10.859375</v>
-      </c>
-      <c r="F11" s="24">
-        <v>1.359375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
-        <v>2.65625</v>
-      </c>
-      <c r="B12" s="24">
-        <v>0.53125</v>
-      </c>
-      <c r="E12" s="24">
-        <v>10.625</v>
-      </c>
-      <c r="F12" s="24">
+      <c r="B14" s="24">
+        <v>0.515625</v>
+      </c>
+      <c r="C14" s="24">
+        <v>0.484375</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="24">
+        <v>9.4375</v>
+      </c>
+      <c r="F14" s="24">
+        <v>1.15625</v>
+      </c>
+      <c r="G14" s="24">
         <v>1.34375</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
-        <v>2.8125</v>
-      </c>
-      <c r="B13" s="24">
-        <v>0.53125</v>
-      </c>
-      <c r="E13" s="24">
-        <v>11.015625</v>
-      </c>
-      <c r="F13" s="24">
-        <v>1.34375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="17" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="19" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="20" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="22" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="23" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="24" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="25" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="26" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="27" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="29" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="30" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="31" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="32" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="34" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="35" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="36" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="37" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="39" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="43" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="46" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="47" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="48" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="49" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="50" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="51" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="52" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="54" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="57" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="58" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="61" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="62" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="63" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="64" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="65" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="66" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="67" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="68" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="69" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="70" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="71" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="72" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="73" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="74" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="75" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="76" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="77" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="78" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="79" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="81" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="82" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="83" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="84" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="85" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="86" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="87" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="88" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="89" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="90" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="91" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="92" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="93" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="94" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="95" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="96" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="24" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B104" s="24" t="s">
+      <c r="B16" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="E104" s="24" t="s">
+      <c r="C16" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="F104" s="24" t="s">
+      <c r="F16" s="26" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="24">
-        <f>SUM(A4:A103)/COUNT(A4:A103)/10</f>
-        <v>0.26734374999999999</v>
-      </c>
-      <c r="B105" s="24">
-        <f>SUM(B4:B103)/COUNT(B4:B103)/100</f>
-        <v>5.3281250000000004E-3</v>
-      </c>
-      <c r="E105" s="24">
-        <f>SUM(E4:E103)/COUNT(E4:E103)</f>
-        <v>10.734375</v>
-      </c>
-      <c r="F105" s="24">
-        <f>SUM(F4:F103)/COUNT(F4:F103)/10</f>
-        <v>0.13468750000000002</v>
+      <c r="G16" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <f>SUM(A5:A14)/COUNT(A5:A14)/10</f>
+        <v>0.26437499999999997</v>
+      </c>
+      <c r="B17" s="27">
+        <f>SUM(B5:B14)/COUNT(B5:B14)/100</f>
+        <v>5.0781250000000002E-3</v>
+      </c>
+      <c r="C17" s="27">
+        <f>SUM(C5:C14)/COUNT(C5:C14)/100</f>
+        <v>4.921875E-3</v>
+      </c>
+      <c r="E17" s="27">
+        <f>SUM(E5:E14)/COUNT(E5:E14)</f>
+        <v>9.1359375000000007</v>
+      </c>
+      <c r="F17" s="27">
+        <f>SUM(F5:F14)/COUNT(F5:F14)/10</f>
+        <v>0.11859375000000001</v>
+      </c>
+      <c r="G17" s="27">
+        <f>SUM(G5:G14)/COUNT(G5:G14)/10</f>
+        <v>0.12250000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>